<commit_message>
updates to source file structures
</commit_message>
<xml_diff>
--- a/effort_source.xlsx
+++ b/effort_source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejnic\Documents\BONWRAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA92A426-F1FE-40AF-BBBF-9B7DAF90B443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C128785-34B6-4D52-9859-F3DC5366F07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{A2B16CEB-D459-4236-98B8-FBEF16A94A9B}"/>
   </bookViews>
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293BC81-D38C-42CF-93E9-1A2FAA41C768}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,236 +481,266 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>7</v>
       </c>
       <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>6</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>18</v>
-      </c>
-      <c r="F2">
-        <v>22</v>
-      </c>
-      <c r="G2">
-        <v>14</v>
-      </c>
-      <c r="H2">
-        <v>14</v>
-      </c>
-      <c r="I2">
-        <v>15</v>
-      </c>
-      <c r="J2">
-        <v>15</v>
-      </c>
-      <c r="K2">
-        <v>13</v>
-      </c>
-      <c r="L2">
-        <v>12</v>
-      </c>
-      <c r="M2">
-        <v>11</v>
-      </c>
-      <c r="N2">
-        <v>12</v>
-      </c>
-      <c r="O2">
-        <v>12</v>
-      </c>
-      <c r="P2">
-        <v>19</v>
-      </c>
-      <c r="Q2">
-        <v>18</v>
-      </c>
-      <c r="R2">
-        <v>16</v>
-      </c>
-      <c r="S2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
       <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
         <v>11</v>
-      </c>
-      <c r="E3">
-        <v>28</v>
-      </c>
-      <c r="F3">
-        <v>18</v>
-      </c>
-      <c r="G3">
-        <v>20.5</v>
-      </c>
-      <c r="H3">
-        <v>19.5</v>
-      </c>
-      <c r="I3">
-        <v>19</v>
-      </c>
-      <c r="J3">
-        <v>25</v>
-      </c>
-      <c r="K3">
-        <v>28</v>
-      </c>
-      <c r="L3">
-        <v>28</v>
-      </c>
-      <c r="M3">
-        <v>22.5</v>
-      </c>
-      <c r="N3">
-        <v>24.5</v>
-      </c>
-      <c r="O3">
-        <v>25.5</v>
-      </c>
-      <c r="P3">
-        <v>25</v>
-      </c>
-      <c r="Q3">
-        <v>28.5</v>
-      </c>
-      <c r="R3">
-        <v>18</v>
-      </c>
-      <c r="S3">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>28</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>20.5</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>19.5</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>28</v>
+      </c>
+      <c r="D11">
         <v>4</v>
       </c>
-      <c r="L4">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>28</v>
+      </c>
+      <c r="D12">
         <v>4</v>
       </c>
-      <c r="M4">
-        <v>3</v>
-      </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="O4">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>22.5</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>24.5</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>25.5</v>
+      </c>
+      <c r="D15">
         <v>4</v>
       </c>
-      <c r="P4">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+      <c r="D16">
         <v>4</v>
       </c>
-      <c r="Q4">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>28.5</v>
+      </c>
+      <c r="D17">
         <v>4</v>
       </c>
-      <c r="R4">
-        <v>3</v>
-      </c>
-      <c r="S4">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>26</v>
+      </c>
+      <c r="D19">
         <v>4</v>
       </c>
     </row>

</xml_diff>